<commit_message>
First version that checks both structure and content of all worksheets of an AEF file
</commit_message>
<xml_diff>
--- a/AEF_files/202504292100---AEF_CMA6_second_iteration - Guyana 2022 correct.xlsx
+++ b/AEF_files/202504292100---AEF_CMA6_second_iteration - Guyana 2022 correct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfccc365.sharepoint.com/sites/Mitigation/Paris Agreement Article 6/Article 6.2/03_CARP/consistency/AEF_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_931399C2B4BF54E2480C1830CFE6AABAECCE8F89" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3099687E-7C90-5640-AF4B-59C50C6A25F2}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="11_931399C2B4BF54E2480C1830CFE6AABAECCE8F89" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B236EA5-6B61-B947-B2A9-FCC4FED6610F}"/>
   <bookViews>
-    <workbookView xWindow="9940" yWindow="2200" windowWidth="39680" windowHeight="19760" tabRatio="618" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9940" yWindow="2200" windowWidth="39680" windowHeight="19760" tabRatio="618" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="165">
   <si>
     <t>Table</t>
   </si>
@@ -625,12 +625,6 @@
     <t>AFOLU</t>
   </si>
   <si>
-    <t>NDC, OIMP, OP</t>
-  </si>
-  <si>
-    <t>First Transfer</t>
-  </si>
-  <si>
     <t>ART 102</t>
   </si>
   <si>
@@ -680,6 +674,12 @@
   </si>
   <si>
     <t>REDD</t>
+  </si>
+  <si>
+    <t>GUY01</t>
+  </si>
+  <si>
+    <t>First transfer</t>
   </si>
 </sst>
 </file>
@@ -687,8 +687,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -1204,17 +1204,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="23" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="18" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1237,14 +1240,11 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="23" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1988,7 +1988,7 @@
         <v>57</v>
       </c>
       <c r="C50" s="74" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="28" x14ac:dyDescent="0.2">
@@ -1996,7 +1996,7 @@
         <v>58</v>
       </c>
       <c r="C51" s="74" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="56" x14ac:dyDescent="0.2">
@@ -2193,7 +2193,7 @@
         <v>57</v>
       </c>
       <c r="C79" s="74" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="28" x14ac:dyDescent="0.2">
@@ -2201,7 +2201,7 @@
         <v>58</v>
       </c>
       <c r="C80" s="74" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="56" x14ac:dyDescent="0.2">
@@ -2217,7 +2217,7 @@
         <v>98</v>
       </c>
       <c r="C82" s="74" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="42" x14ac:dyDescent="0.2">
@@ -2225,7 +2225,7 @@
         <v>99</v>
       </c>
       <c r="C83" s="74" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.2">
@@ -2404,8 +2404,8 @@
       <c r="B5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="99" t="s">
-        <v>160</v>
+      <c r="C5" s="90" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
@@ -2420,7 +2420,7 @@
       <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="98">
+      <c r="C7" s="89">
         <v>45904</v>
       </c>
     </row>
@@ -2465,8 +2465,8 @@
       </c>
     </row>
     <row r="13" spans="2:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="91"/>
-      <c r="C13" s="91"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2481,7 +2481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
@@ -2518,12 +2518,12 @@
       </c>
     </row>
     <row r="5" spans="2:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
       <c r="F5" s="33"/>
       <c r="G5" s="34" t="s">
         <v>44</v>
@@ -2627,9 +2627,9 @@
     </row>
     <row r="8" spans="2:21" ht="152.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="81" t="s">
-        <v>150</v>
-      </c>
-      <c r="C8" s="100">
+        <v>148</v>
+      </c>
+      <c r="C8" s="91">
         <v>45707</v>
       </c>
       <c r="D8" s="82" t="s">
@@ -2655,24 +2655,24 @@
         <v>145</v>
       </c>
       <c r="L8" s="85" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="M8" s="86" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="N8" s="81" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O8" s="19"/>
       <c r="P8" s="81" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="R8" s="19"/>
       <c r="S8" s="57" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="T8" s="24" t="s">
         <v>10</v>
@@ -2822,13 +2822,13 @@
   <dimension ref="B3:AH13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH8" sqref="AH8"/>
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="15"/>
-    <col min="2" max="2" width="8.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" style="15" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" style="15" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" style="15" bestFit="1" customWidth="1"/>
@@ -2978,17 +2978,17 @@
       <c r="V6" s="38"/>
       <c r="W6" s="38"/>
       <c r="X6" s="36"/>
-      <c r="Y6" s="94" t="s">
+      <c r="Y6" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="Z6" s="94"/>
+      <c r="Z6" s="95"/>
       <c r="AA6" s="40"/>
-      <c r="AB6" s="93" t="s">
+      <c r="AB6" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="AC6" s="93"/>
-      <c r="AD6" s="93"/>
-      <c r="AE6" s="93"/>
+      <c r="AC6" s="94"/>
+      <c r="AD6" s="94"/>
+      <c r="AE6" s="94"/>
       <c r="AF6" s="36"/>
       <c r="AG6" s="23"/>
       <c r="AH6" s="23"/>
@@ -3122,11 +3122,11 @@
       </c>
     </row>
     <row r="9" spans="2:34" ht="56" x14ac:dyDescent="0.2">
-      <c r="B9" s="87">
+      <c r="B9" s="99">
         <v>45292</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>20</v>
@@ -3135,29 +3135,29 @@
         <v>144</v>
       </c>
       <c r="F9" s="81" t="s">
+        <v>148</v>
+      </c>
+      <c r="G9" s="81" t="s">
+        <v>160</v>
+      </c>
+      <c r="H9" s="81" t="s">
+        <v>163</v>
+      </c>
+      <c r="I9" s="87" t="s">
+        <v>149</v>
+      </c>
+      <c r="J9" s="88" t="s">
         <v>150</v>
-      </c>
-      <c r="G9" s="81" t="s">
-        <v>150</v>
-      </c>
-      <c r="H9" s="81" t="s">
-        <v>150</v>
-      </c>
-      <c r="I9" s="88" t="s">
-        <v>151</v>
-      </c>
-      <c r="J9" s="89" t="s">
-        <v>152</v>
       </c>
       <c r="K9" s="19"/>
       <c r="L9" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="M9" s="82" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N9" s="82" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="O9" s="19"/>
       <c r="P9" s="24" t="s">
@@ -3182,13 +3182,11 @@
       </c>
       <c r="X9" s="19"/>
       <c r="Y9" s="81" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="Z9" s="46"/>
       <c r="AA9" s="46"/>
-      <c r="AB9" s="86" t="s">
-        <v>146</v>
-      </c>
+      <c r="AB9" s="86"/>
       <c r="AC9" s="44"/>
       <c r="AD9" s="44"/>
       <c r="AE9" s="44"/>
@@ -3339,7 +3337,7 @@
   <dimension ref="B3:U34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3367,54 +3365,54 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
-      <c r="H3" s="96"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
       <c r="L3" s="50"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="98"/>
+      <c r="R3" s="98"/>
+      <c r="S3" s="98"/>
+      <c r="T3" s="98"/>
     </row>
     <row r="4" spans="2:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="66"/>
       <c r="C4" s="67"/>
       <c r="D4" s="68"/>
       <c r="E4" s="67"/>
-      <c r="F4" s="95" t="s">
+      <c r="F4" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
       <c r="L4" s="69"/>
-      <c r="M4" s="95" t="s">
+      <c r="M4" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="95"/>
-      <c r="O4" s="95"/>
-      <c r="P4" s="95"/>
-      <c r="Q4" s="95"/>
+      <c r="N4" s="96"/>
+      <c r="O4" s="96"/>
+      <c r="P4" s="96"/>
+      <c r="Q4" s="96"/>
       <c r="R4" s="69"/>
-      <c r="S4" s="95" t="s">
+      <c r="S4" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="T4" s="95"/>
+      <c r="T4" s="96"/>
       <c r="U4" s="36"/>
     </row>
     <row r="5" spans="2:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3422,16 +3420,16 @@
       <c r="C5" s="23"/>
       <c r="D5" s="38"/>
       <c r="E5" s="38"/>
-      <c r="F5" s="93" t="s">
+      <c r="F5" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="93"/>
+      <c r="G5" s="94"/>
       <c r="H5" s="18"/>
-      <c r="I5" s="93" t="s">
+      <c r="I5" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
       <c r="L5" s="18"/>
       <c r="M5" s="38"/>
       <c r="N5" s="38"/>
@@ -3452,10 +3450,10 @@
       <c r="G6" s="37"/>
       <c r="H6" s="18"/>
       <c r="I6" s="23"/>
-      <c r="J6" s="93" t="s">
+      <c r="J6" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="93"/>
+      <c r="K6" s="94"/>
       <c r="L6" s="18"/>
       <c r="M6" s="38"/>
       <c r="N6" s="38"/>
@@ -3526,29 +3524,29 @@
         <v>144</v>
       </c>
       <c r="C8" s="81" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="81" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="81" t="s">
+        <v>163</v>
+      </c>
+      <c r="F8" s="87" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" s="88" t="s">
         <v>150</v>
-      </c>
-      <c r="D8" s="81" t="s">
-        <v>150</v>
-      </c>
-      <c r="E8" s="81" t="s">
-        <v>150</v>
-      </c>
-      <c r="F8" s="88" t="s">
-        <v>151</v>
-      </c>
-      <c r="G8" s="89" t="s">
-        <v>152</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J8" s="82" t="s">
+        <v>151</v>
+      </c>
+      <c r="K8" s="82" t="s">
         <v>153</v>
-      </c>
-      <c r="K8" s="82" t="s">
-        <v>155</v>
       </c>
       <c r="L8" s="19"/>
       <c r="M8" s="19" t="s">
@@ -3999,8 +3997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C8:K13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4023,11 +4021,11 @@
     </row>
     <row r="9" spans="3:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="51"/>
-      <c r="D9" s="93" t="s">
+      <c r="D9" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
       <c r="G9" s="52"/>
       <c r="H9" s="51"/>
       <c r="I9" s="51"/>
@@ -4062,7 +4060,7 @@
       <c r="K10" s="53"/>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C11" s="90">
+      <c r="C11" s="100">
         <v>45707</v>
       </c>
       <c r="D11" s="53"/>
@@ -4099,6 +4097,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="819ae873-75e1-413b-9d00-7af9258cf281">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="eb4559c4-8463-4985-927f-f0d558bff8f0" xsi:nil="true"/>
+    <Ready xmlns="819ae873-75e1-413b-9d00-7af9258cf281">true</Ready>
+    <Comments xmlns="819ae873-75e1-413b-9d00-7af9258cf281" xsi:nil="true"/>
+    <Doc_x002e_SymbolNumber xmlns="819ae873-75e1-413b-9d00-7af9258cf281" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="819ae873-75e1-413b-9d00-7af9258cf281" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="9d8c265a-5436-43a7-80c1-713d2827ffde" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FB6730B0802B54A9F00C78B857E1443" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3aa8ea1b9f2e27c2fdef6ef4056186e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="819ae873-75e1-413b-9d00-7af9258cf281" xmlns:ns3="eb4559c4-8463-4985-927f-f0d558bff8f0" xmlns:ns4="13d80b15-5f07-43ab-b435-85767a7dac08" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="16259e29b70fac56f05f7b64cc1f875d" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="819ae873-75e1-413b-9d00-7af9258cf281"/>
@@ -4380,36 +4407,41 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="9d8c265a-5436-43a7-80c1-713d2827ffde" ContentTypeId="0x0101" PreviousValue="false"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9846E218-2C67-4B45-A7CB-841EE05F366A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="819ae873-75e1-413b-9d00-7af9258cf281">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="eb4559c4-8463-4985-927f-f0d558bff8f0" xsi:nil="true"/>
-    <Ready xmlns="819ae873-75e1-413b-9d00-7af9258cf281">true</Ready>
-    <Comments xmlns="819ae873-75e1-413b-9d00-7af9258cf281" xsi:nil="true"/>
-    <Doc_x002e_SymbolNumber xmlns="819ae873-75e1-413b-9d00-7af9258cf281" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="819ae873-75e1-413b-9d00-7af9258cf281" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17AB3B8A-2D8D-4EE0-964D-A16E3E636991}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="eb4559c4-8463-4985-927f-f0d558bff8f0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="13d80b15-5f07-43ab-b435-85767a7dac08"/>
+    <ds:schemaRef ds:uri="819ae873-75e1-413b-9d00-7af9258cf281"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A37B77DB-672E-4904-BCCD-9AB8AC3DE6E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D315F9A0-41BA-46E2-9C24-0BDD84BA9037}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4427,38 +4459,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A37B77DB-672E-4904-BCCD-9AB8AC3DE6E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17AB3B8A-2D8D-4EE0-964D-A16E3E636991}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="eb4559c4-8463-4985-927f-f0d558bff8f0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="819ae873-75e1-413b-9d00-7af9258cf281"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="13d80b15-5f07-43ab-b435-85767a7dac08"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9846E218-2C67-4B45-A7CB-841EE05F366A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>